<commit_message>
"Exportando datos a excel(incompleto)"
</commit_message>
<xml_diff>
--- a/Formato desglose.xlsx
+++ b/Formato desglose.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24930" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="datos" sheetId="2" r:id="rId1"/>
@@ -90,7 +90,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +146,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial Narrow"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -332,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -415,6 +422,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -721,9 +732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -745,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,7 +786,7 @@
       <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="25" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="6"/>
@@ -877,16 +886,25 @@
       <c r="A6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="24"/>
+      <c r="B6" s="24">
+        <f>datos!C2</f>
+        <v>0</v>
+      </c>
       <c r="D6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="24"/>
+      <c r="E6" s="24">
+        <f>datos!C4</f>
+        <v>0</v>
+      </c>
       <c r="F6" s="4"/>
       <c r="G6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="24"/>
+      <c r="H6" s="24">
+        <f>datos!C6</f>
+        <v>0</v>
+      </c>
       <c r="I6" s="4"/>
       <c r="J6" s="16"/>
       <c r="K6" s="12"/>
@@ -895,16 +913,25 @@
       <c r="A7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="18"/>
+      <c r="B7" s="18">
+        <f>datos!D2</f>
+        <v>0</v>
+      </c>
       <c r="D7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="18"/>
+      <c r="E7" s="18">
+        <f>datos!D4</f>
+        <v>0</v>
+      </c>
       <c r="F7" s="4"/>
       <c r="G7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="18"/>
+      <c r="H7" s="18">
+        <f>datos!D6</f>
+        <v>0</v>
+      </c>
       <c r="I7" s="4"/>
       <c r="J7" s="16"/>
       <c r="K7" s="12"/>
@@ -913,16 +940,25 @@
       <c r="A8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="24"/>
+      <c r="B8" s="24">
+        <f>datos!E2</f>
+        <v>0</v>
+      </c>
       <c r="D8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="24"/>
+      <c r="E8" s="24">
+        <f>datos!E4</f>
+        <v>0</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="24"/>
+      <c r="H8" s="24">
+        <f>datos!E6</f>
+        <v>0</v>
+      </c>
       <c r="I8" s="4"/>
       <c r="J8" s="16"/>
       <c r="K8" s="12"/>
@@ -931,16 +967,25 @@
       <c r="A9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="18"/>
+      <c r="B9" s="18">
+        <f>datos!F2</f>
+        <v>0</v>
+      </c>
       <c r="D9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="18"/>
+      <c r="E9" s="18">
+        <f>datos!F4</f>
+        <v>0</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="18"/>
+      <c r="H9" s="18">
+        <f>datos!F6</f>
+        <v>0</v>
+      </c>
       <c r="I9" s="4"/>
       <c r="J9" s="16"/>
       <c r="K9" s="12"/>
@@ -949,16 +994,25 @@
       <c r="A10" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="24"/>
+      <c r="B10" s="24">
+        <f>datos!G2</f>
+        <v>0</v>
+      </c>
       <c r="D10" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="24"/>
+      <c r="E10" s="24">
+        <f>datos!G4</f>
+        <v>0</v>
+      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="24"/>
+      <c r="H10" s="24">
+        <f>datos!G6</f>
+        <v>0</v>
+      </c>
       <c r="I10" s="4"/>
       <c r="J10" s="16"/>
       <c r="K10" s="12"/>
@@ -967,16 +1021,25 @@
       <c r="A11" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="20"/>
+      <c r="B11" s="20">
+        <f>datos!H2</f>
+        <v>0</v>
+      </c>
       <c r="D11" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="20"/>
+      <c r="E11" s="20">
+        <f>datos!H4</f>
+        <v>0</v>
+      </c>
       <c r="F11" s="4"/>
       <c r="G11" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="20"/>
+      <c r="H11" s="20">
+        <f>datos!H6</f>
+        <v>0</v>
+      </c>
       <c r="I11" s="4"/>
       <c r="J11" s="16"/>
       <c r="K11" s="12"/>
@@ -1075,92 +1138,146 @@
       <c r="A16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="24"/>
+      <c r="B16" s="24">
+        <f>datos!C8</f>
+        <v>0</v>
+      </c>
       <c r="D16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="24"/>
+      <c r="E16" s="24">
+        <f>datos!C10</f>
+        <v>0</v>
+      </c>
       <c r="F16" s="4"/>
       <c r="G16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="24"/>
+      <c r="H16" s="24">
+        <f>datos!C12</f>
+        <v>0</v>
+      </c>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="18"/>
+      <c r="B17" s="18">
+        <f>datos!D8</f>
+        <v>0</v>
+      </c>
       <c r="D17" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="18"/>
+      <c r="E17" s="18">
+        <f>datos!D10</f>
+        <v>0</v>
+      </c>
       <c r="F17" s="4"/>
       <c r="G17" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="18"/>
+      <c r="H17" s="18">
+        <f>datos!D12</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="24"/>
+      <c r="B18" s="24">
+        <f>datos!E8</f>
+        <v>0</v>
+      </c>
       <c r="D18" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="24"/>
+      <c r="E18" s="24">
+        <f>datos!E10</f>
+        <v>0</v>
+      </c>
       <c r="F18" s="4"/>
       <c r="G18" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="H18" s="24"/>
+      <c r="H18" s="24">
+        <f>datos!E12</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="18"/>
+      <c r="B19" s="18">
+        <f>datos!F4</f>
+        <v>0</v>
+      </c>
       <c r="D19" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="18"/>
+      <c r="E19" s="18">
+        <f>datos!F10</f>
+        <v>0</v>
+      </c>
       <c r="F19" s="4"/>
       <c r="G19" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H19" s="18"/>
+      <c r="H19" s="18">
+        <f>datos!F12</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="24"/>
+      <c r="B20" s="24">
+        <f>datos!G8</f>
+        <v>0</v>
+      </c>
       <c r="D20" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="24"/>
+      <c r="E20" s="24">
+        <f>datos!G10</f>
+        <v>0</v>
+      </c>
       <c r="F20" s="4"/>
       <c r="G20" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="24"/>
+      <c r="H20" s="24">
+        <f>datos!G12</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="20"/>
+      <c r="B21" s="20">
+        <f>datos!H8</f>
+        <v>0</v>
+      </c>
       <c r="D21" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="20"/>
+      <c r="E21" s="20">
+        <f>datos!H10</f>
+        <v>0</v>
+      </c>
       <c r="F21" s="4"/>
       <c r="G21" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="20"/>
+      <c r="H21" s="20">
+        <f>datos!H12</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -1251,91 +1368,145 @@
       <c r="A26" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="24"/>
+      <c r="B26" s="24">
+        <f>datos!C14</f>
+        <v>0</v>
+      </c>
       <c r="D26" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="24"/>
+      <c r="E26" s="24">
+        <f>datos!C16</f>
+        <v>0</v>
+      </c>
       <c r="F26" s="4"/>
       <c r="G26" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="24"/>
+      <c r="H26" s="24">
+        <f>datos!C18</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="18"/>
+      <c r="B27" s="18">
+        <f>datos!D14</f>
+        <v>0</v>
+      </c>
       <c r="D27" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="18"/>
+      <c r="E27" s="18">
+        <f>datos!D16</f>
+        <v>0</v>
+      </c>
       <c r="F27" s="4"/>
       <c r="G27" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H27" s="18"/>
+      <c r="H27" s="18">
+        <f>datos!D18</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="24"/>
+      <c r="B28" s="24">
+        <f>datos!E14</f>
+        <v>0</v>
+      </c>
       <c r="D28" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="24"/>
+      <c r="E28" s="24">
+        <f>datos!E16</f>
+        <v>0</v>
+      </c>
       <c r="F28" s="4"/>
       <c r="G28" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="H28" s="24"/>
+      <c r="H28" s="24">
+        <f>datos!E18</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="18"/>
+      <c r="B29" s="18">
+        <f>datos!F14</f>
+        <v>0</v>
+      </c>
       <c r="D29" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="18"/>
+      <c r="E29" s="18">
+        <f>datos!F16</f>
+        <v>0</v>
+      </c>
       <c r="F29" s="4"/>
       <c r="G29" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H29" s="18"/>
+      <c r="H29" s="18">
+        <f>datos!F18</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="24"/>
+      <c r="B30" s="24">
+        <f>datos!G14</f>
+        <v>0</v>
+      </c>
       <c r="D30" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="24"/>
+      <c r="E30" s="24">
+        <f>datos!G16</f>
+        <v>0</v>
+      </c>
       <c r="F30" s="4"/>
       <c r="G30" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H30" s="24"/>
+      <c r="H30" s="24">
+        <f>datos!G18</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="20"/>
+      <c r="B31" s="20">
+        <f>datos!H14</f>
+        <v>0</v>
+      </c>
       <c r="D31" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="20"/>
+      <c r="E31" s="20">
+        <f>datos!H16</f>
+        <v>0</v>
+      </c>
       <c r="F31" s="4"/>
       <c r="G31" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H31" s="20"/>
+      <c r="H31" s="20">
+        <f>datos!H18</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
@@ -1426,91 +1597,145 @@
       <c r="A36" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="24"/>
+      <c r="B36" s="24">
+        <f>datos!C20</f>
+        <v>0</v>
+      </c>
       <c r="D36" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E36" s="24"/>
+      <c r="E36" s="24">
+        <f>datos!C22</f>
+        <v>0</v>
+      </c>
       <c r="F36" s="4"/>
       <c r="G36" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H36" s="24"/>
+      <c r="H36" s="24">
+        <f>datos!C24</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B37" s="18"/>
+      <c r="B37" s="18">
+        <f>datos!D20</f>
+        <v>0</v>
+      </c>
       <c r="D37" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="18"/>
+      <c r="E37" s="18">
+        <f>datos!D22</f>
+        <v>0</v>
+      </c>
       <c r="F37" s="4"/>
       <c r="G37" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H37" s="18"/>
+      <c r="H37" s="18">
+        <f>datos!D24</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="24"/>
+      <c r="B38" s="24">
+        <f>datos!E20</f>
+        <v>0</v>
+      </c>
       <c r="D38" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E38" s="24"/>
+      <c r="E38" s="24">
+        <f>datos!E22</f>
+        <v>0</v>
+      </c>
       <c r="F38" s="4"/>
       <c r="G38" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="H38" s="24"/>
+      <c r="H38" s="24">
+        <f>datos!E24</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="18"/>
+      <c r="B39" s="18">
+        <f>datos!F20</f>
+        <v>0</v>
+      </c>
       <c r="D39" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E39" s="18"/>
+      <c r="E39" s="18">
+        <f>datos!F22</f>
+        <v>0</v>
+      </c>
       <c r="F39" s="4"/>
       <c r="G39" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H39" s="18"/>
+      <c r="H39" s="18">
+        <f>datos!F24</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="24"/>
+      <c r="B40" s="24">
+        <f>datos!G20</f>
+        <v>0</v>
+      </c>
       <c r="D40" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="24"/>
+      <c r="E40" s="24">
+        <f>datos!G22</f>
+        <v>0</v>
+      </c>
       <c r="F40" s="4"/>
       <c r="G40" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H40" s="24"/>
+      <c r="H40" s="24">
+        <f>datos!G24</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="20"/>
+      <c r="B41" s="20">
+        <f>datos!H20</f>
+        <v>0</v>
+      </c>
       <c r="D41" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E41" s="20"/>
+      <c r="E41" s="20">
+        <f>datos!H22</f>
+        <v>0</v>
+      </c>
       <c r="F41" s="4"/>
       <c r="G41" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H41" s="20"/>
+      <c r="H41" s="20">
+        <f>datos!H24</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
@@ -1578,7 +1803,7 @@
   <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1709,16 +1934,25 @@
       <c r="A6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="24"/>
+      <c r="B6" s="24">
+        <f>datos!C26</f>
+        <v>0</v>
+      </c>
       <c r="D6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="24"/>
+      <c r="E6" s="24">
+        <f>datos!C28</f>
+        <v>0</v>
+      </c>
       <c r="F6" s="4"/>
       <c r="G6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="24"/>
+      <c r="H6" s="24">
+        <f>datos!C30</f>
+        <v>0</v>
+      </c>
       <c r="I6" s="4"/>
       <c r="J6" s="16"/>
       <c r="K6" s="12"/>
@@ -1727,16 +1961,25 @@
       <c r="A7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="18"/>
+      <c r="B7" s="18">
+        <f>datos!D26</f>
+        <v>0</v>
+      </c>
       <c r="D7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="18"/>
+      <c r="E7" s="18">
+        <f>datos!D28</f>
+        <v>0</v>
+      </c>
       <c r="F7" s="4"/>
       <c r="G7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="18"/>
+      <c r="H7" s="18">
+        <f>datos!D30</f>
+        <v>0</v>
+      </c>
       <c r="I7" s="4"/>
       <c r="J7" s="16"/>
       <c r="K7" s="12"/>
@@ -1745,16 +1988,25 @@
       <c r="A8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="24"/>
+      <c r="B8" s="24">
+        <f>datos!E26</f>
+        <v>0</v>
+      </c>
       <c r="D8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="24"/>
+      <c r="E8" s="24">
+        <f>datos!E28</f>
+        <v>0</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="24"/>
+      <c r="H8" s="24">
+        <f>datos!E30</f>
+        <v>0</v>
+      </c>
       <c r="I8" s="4"/>
       <c r="J8" s="16"/>
       <c r="K8" s="12"/>
@@ -1763,16 +2015,25 @@
       <c r="A9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="18"/>
+      <c r="B9" s="18">
+        <f>datos!F26</f>
+        <v>0</v>
+      </c>
       <c r="D9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="18"/>
+      <c r="E9" s="18">
+        <f>datos!F28</f>
+        <v>0</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="18"/>
+      <c r="H9" s="18">
+        <f>datos!F30</f>
+        <v>0</v>
+      </c>
       <c r="I9" s="4"/>
       <c r="J9" s="16"/>
       <c r="K9" s="12"/>
@@ -1781,16 +2042,25 @@
       <c r="A10" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="24"/>
+      <c r="B10" s="24">
+        <f>datos!G26</f>
+        <v>0</v>
+      </c>
       <c r="D10" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="24"/>
+      <c r="E10" s="24">
+        <f>datos!G28</f>
+        <v>0</v>
+      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="24"/>
+      <c r="H10" s="24">
+        <f>datos!G30</f>
+        <v>0</v>
+      </c>
       <c r="I10" s="4"/>
       <c r="J10" s="16"/>
       <c r="K10" s="12"/>
@@ -1799,16 +2069,25 @@
       <c r="A11" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="20"/>
+      <c r="B11" s="20">
+        <f>datos!H26</f>
+        <v>0</v>
+      </c>
       <c r="D11" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="20"/>
+      <c r="E11" s="20">
+        <f>datos!H28</f>
+        <v>0</v>
+      </c>
       <c r="F11" s="4"/>
       <c r="G11" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="20"/>
+      <c r="H11" s="20">
+        <f>datos!H30</f>
+        <v>0</v>
+      </c>
       <c r="I11" s="4"/>
       <c r="J11" s="16"/>
       <c r="K11" s="12"/>
@@ -1907,92 +2186,146 @@
       <c r="A16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="24"/>
+      <c r="B16" s="24">
+        <f>datos!C30</f>
+        <v>0</v>
+      </c>
       <c r="D16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="24"/>
+      <c r="E16" s="24">
+        <f>datos!C34</f>
+        <v>0</v>
+      </c>
       <c r="F16" s="4"/>
       <c r="G16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="24"/>
+      <c r="H16" s="24">
+        <f>datos!C36</f>
+        <v>0</v>
+      </c>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="18"/>
+      <c r="B17" s="24">
+        <f>datos!D30</f>
+        <v>0</v>
+      </c>
       <c r="D17" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="18"/>
+      <c r="E17" s="24">
+        <f>datos!D34</f>
+        <v>0</v>
+      </c>
       <c r="F17" s="4"/>
       <c r="G17" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="18"/>
+      <c r="H17" s="24">
+        <f>datos!D36</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="24"/>
+      <c r="B18" s="24">
+        <f>datos!E30</f>
+        <v>0</v>
+      </c>
       <c r="D18" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="24"/>
+      <c r="E18" s="24">
+        <f>datos!E34</f>
+        <v>0</v>
+      </c>
       <c r="F18" s="4"/>
       <c r="G18" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="H18" s="24"/>
+      <c r="H18" s="24">
+        <f>datos!E36</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="18"/>
+      <c r="B19" s="24">
+        <f>datos!F30</f>
+        <v>0</v>
+      </c>
       <c r="D19" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="18"/>
+      <c r="E19" s="24">
+        <f>datos!F34</f>
+        <v>0</v>
+      </c>
       <c r="F19" s="4"/>
       <c r="G19" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H19" s="18"/>
+      <c r="H19" s="24">
+        <f>datos!F36</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="24"/>
+      <c r="B20" s="24">
+        <f>datos!G30</f>
+        <v>0</v>
+      </c>
       <c r="D20" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="24"/>
+      <c r="E20" s="24">
+        <f>datos!G34</f>
+        <v>0</v>
+      </c>
       <c r="F20" s="4"/>
       <c r="G20" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="24"/>
+      <c r="H20" s="24">
+        <f>datos!G36</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="20"/>
+      <c r="B21" s="24">
+        <f>datos!H30</f>
+        <v>0</v>
+      </c>
       <c r="D21" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="20"/>
+      <c r="E21" s="24">
+        <f>datos!H34</f>
+        <v>0</v>
+      </c>
       <c r="F21" s="4"/>
       <c r="G21" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="20"/>
+      <c r="H21" s="24">
+        <f>datos!H36</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
@@ -2083,91 +2416,145 @@
       <c r="A26" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="24"/>
+      <c r="B26" s="24">
+        <f>datos!C38</f>
+        <v>0</v>
+      </c>
       <c r="D26" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="24"/>
+      <c r="E26" s="24">
+        <f>datos!C40</f>
+        <v>0</v>
+      </c>
       <c r="F26" s="4"/>
       <c r="G26" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="24"/>
+      <c r="H26" s="24">
+        <f>datos!C42</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="18"/>
+      <c r="B27" s="24">
+        <f>datos!D38</f>
+        <v>0</v>
+      </c>
       <c r="D27" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="18"/>
+      <c r="E27" s="24">
+        <f>datos!D40</f>
+        <v>0</v>
+      </c>
       <c r="F27" s="4"/>
       <c r="G27" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H27" s="18"/>
+      <c r="H27" s="24">
+        <f>datos!D42</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="24"/>
+      <c r="B28" s="24">
+        <f>datos!E38</f>
+        <v>0</v>
+      </c>
       <c r="D28" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="24"/>
+      <c r="E28" s="24">
+        <f>datos!E40</f>
+        <v>0</v>
+      </c>
       <c r="F28" s="4"/>
       <c r="G28" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="H28" s="24"/>
+      <c r="H28" s="24">
+        <f>datos!E42</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="18"/>
+      <c r="B29" s="24">
+        <f>datos!F38</f>
+        <v>0</v>
+      </c>
       <c r="D29" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="18"/>
+      <c r="E29" s="24">
+        <f>datos!F40</f>
+        <v>0</v>
+      </c>
       <c r="F29" s="4"/>
       <c r="G29" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H29" s="18"/>
+      <c r="H29" s="24">
+        <f>datos!F42</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="24"/>
+      <c r="B30" s="24">
+        <f>datos!G38</f>
+        <v>0</v>
+      </c>
       <c r="D30" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="24"/>
+      <c r="E30" s="24">
+        <f>datos!G40</f>
+        <v>0</v>
+      </c>
       <c r="F30" s="4"/>
       <c r="G30" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H30" s="24"/>
+      <c r="H30" s="24">
+        <f>datos!G42</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="20"/>
+      <c r="B31" s="24">
+        <f>datos!H38</f>
+        <v>0</v>
+      </c>
       <c r="D31" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="20"/>
+      <c r="E31" s="24">
+        <f>datos!H40</f>
+        <v>0</v>
+      </c>
       <c r="F31" s="4"/>
       <c r="G31" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H31" s="20"/>
+      <c r="H31" s="24">
+        <f>datos!H42</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
@@ -2258,91 +2645,145 @@
       <c r="A36" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="24"/>
+      <c r="B36" s="24">
+        <f>datos!C44</f>
+        <v>0</v>
+      </c>
       <c r="D36" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E36" s="24"/>
+      <c r="E36" s="24">
+        <f>datos!C46</f>
+        <v>0</v>
+      </c>
       <c r="F36" s="4"/>
       <c r="G36" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H36" s="24"/>
+      <c r="H36" s="24">
+        <f>datos!C48</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B37" s="18"/>
+      <c r="B37" s="24">
+        <f>datos!D44</f>
+        <v>0</v>
+      </c>
       <c r="D37" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="18"/>
+      <c r="E37" s="24">
+        <f>datos!D46</f>
+        <v>0</v>
+      </c>
       <c r="F37" s="4"/>
       <c r="G37" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H37" s="18"/>
+      <c r="H37" s="24">
+        <f>datos!D48</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="24"/>
+      <c r="B38" s="24">
+        <f>datos!E44</f>
+        <v>0</v>
+      </c>
       <c r="D38" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E38" s="24"/>
+      <c r="E38" s="24">
+        <f>datos!E46</f>
+        <v>0</v>
+      </c>
       <c r="F38" s="4"/>
       <c r="G38" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="H38" s="24"/>
+      <c r="H38" s="24">
+        <f>datos!E48</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="18"/>
+      <c r="B39" s="24">
+        <f>datos!F44</f>
+        <v>0</v>
+      </c>
       <c r="D39" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E39" s="18"/>
+      <c r="E39" s="24">
+        <f>datos!F46</f>
+        <v>0</v>
+      </c>
       <c r="F39" s="4"/>
       <c r="G39" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H39" s="18"/>
+      <c r="H39" s="24">
+        <f>datos!F48</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="24"/>
+      <c r="B40" s="24">
+        <f>datos!G44</f>
+        <v>0</v>
+      </c>
       <c r="D40" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="24"/>
+      <c r="E40" s="24">
+        <f>datos!G46</f>
+        <v>0</v>
+      </c>
       <c r="F40" s="4"/>
       <c r="G40" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H40" s="24"/>
+      <c r="H40" s="24">
+        <f>datos!G48</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="20"/>
+      <c r="B41" s="24">
+        <f>datos!H44</f>
+        <v>0</v>
+      </c>
       <c r="D41" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E41" s="20"/>
+      <c r="E41" s="24">
+        <f>datos!H46</f>
+        <v>0</v>
+      </c>
       <c r="F41" s="4"/>
       <c r="G41" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H41" s="20"/>
+      <c r="H41" s="24">
+        <f>datos!H48</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
@@ -2409,8 +2850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2541,16 +2982,25 @@
       <c r="A6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="24"/>
+      <c r="B6" s="24">
+        <f>datos!C50</f>
+        <v>0</v>
+      </c>
       <c r="D6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="24"/>
+      <c r="E6" s="24">
+        <f>datos!C52</f>
+        <v>0</v>
+      </c>
       <c r="F6" s="4"/>
       <c r="G6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="24"/>
+      <c r="H6" s="24">
+        <f>datos!C54</f>
+        <v>0</v>
+      </c>
       <c r="I6" s="4"/>
       <c r="J6" s="16"/>
       <c r="K6" s="12"/>
@@ -2559,16 +3009,25 @@
       <c r="A7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="18"/>
+      <c r="B7" s="24">
+        <f>datos!D50</f>
+        <v>0</v>
+      </c>
       <c r="D7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="18"/>
+      <c r="E7" s="24">
+        <f>datos!D52</f>
+        <v>0</v>
+      </c>
       <c r="F7" s="4"/>
       <c r="G7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="18"/>
+      <c r="H7" s="24">
+        <f>datos!D54</f>
+        <v>0</v>
+      </c>
       <c r="I7" s="4"/>
       <c r="J7" s="16"/>
       <c r="K7" s="12"/>
@@ -2577,16 +3036,25 @@
       <c r="A8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="24"/>
+      <c r="B8" s="24">
+        <f>datos!E50</f>
+        <v>0</v>
+      </c>
       <c r="D8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="24"/>
+      <c r="E8" s="24">
+        <f>datos!E52</f>
+        <v>0</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="24"/>
+      <c r="H8" s="24">
+        <f>datos!E54</f>
+        <v>0</v>
+      </c>
       <c r="I8" s="4"/>
       <c r="J8" s="16"/>
       <c r="K8" s="12"/>
@@ -2595,16 +3063,25 @@
       <c r="A9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="18"/>
+      <c r="B9" s="24">
+        <f>datos!F50</f>
+        <v>0</v>
+      </c>
       <c r="D9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="18"/>
+      <c r="E9" s="24">
+        <f>datos!F52</f>
+        <v>0</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="18"/>
+      <c r="H9" s="24">
+        <f>datos!F54</f>
+        <v>0</v>
+      </c>
       <c r="I9" s="4"/>
       <c r="J9" s="16"/>
       <c r="K9" s="12"/>
@@ -2613,16 +3090,25 @@
       <c r="A10" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="24"/>
+      <c r="B10" s="24">
+        <f>datos!G50</f>
+        <v>0</v>
+      </c>
       <c r="D10" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="24"/>
+      <c r="E10" s="24">
+        <f>datos!G52</f>
+        <v>0</v>
+      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="24"/>
+      <c r="H10" s="24">
+        <f>datos!G54</f>
+        <v>0</v>
+      </c>
       <c r="I10" s="4"/>
       <c r="J10" s="16"/>
       <c r="K10" s="12"/>
@@ -2631,16 +3117,25 @@
       <c r="A11" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="20"/>
+      <c r="B11" s="24">
+        <f>datos!H50</f>
+        <v>0</v>
+      </c>
       <c r="D11" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="20"/>
+      <c r="E11" s="24">
+        <f>datos!H52</f>
+        <v>0</v>
+      </c>
       <c r="F11" s="4"/>
       <c r="G11" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="20"/>
+      <c r="H11" s="24">
+        <f>datos!H54</f>
+        <v>0</v>
+      </c>
       <c r="I11" s="4"/>
       <c r="J11" s="16"/>
       <c r="K11" s="12"/>
@@ -2739,92 +3234,146 @@
       <c r="A16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="24"/>
+      <c r="B16" s="24">
+        <f>datos!C56</f>
+        <v>0</v>
+      </c>
       <c r="D16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="24"/>
+      <c r="E16" s="24">
+        <f>datos!C58</f>
+        <v>0</v>
+      </c>
       <c r="F16" s="4"/>
       <c r="G16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="24"/>
+      <c r="H16" s="24">
+        <f>datos!C60</f>
+        <v>0</v>
+      </c>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="18"/>
+      <c r="B17" s="24">
+        <f>datos!D56</f>
+        <v>0</v>
+      </c>
       <c r="D17" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="18"/>
+      <c r="E17" s="24">
+        <f>datos!D58</f>
+        <v>0</v>
+      </c>
       <c r="F17" s="4"/>
       <c r="G17" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="18"/>
+      <c r="H17" s="24">
+        <f>datos!D60</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="24"/>
+      <c r="B18" s="24">
+        <f>datos!E56</f>
+        <v>0</v>
+      </c>
       <c r="D18" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="24"/>
+      <c r="E18" s="24">
+        <f>datos!E58</f>
+        <v>0</v>
+      </c>
       <c r="F18" s="4"/>
       <c r="G18" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="H18" s="24"/>
+      <c r="H18" s="24">
+        <f>datos!E60</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="18"/>
+      <c r="B19" s="24">
+        <f>datos!F56</f>
+        <v>0</v>
+      </c>
       <c r="D19" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="18"/>
+      <c r="E19" s="24">
+        <f>datos!F58</f>
+        <v>0</v>
+      </c>
       <c r="F19" s="4"/>
       <c r="G19" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H19" s="18"/>
+      <c r="H19" s="24">
+        <f>datos!F60</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="24"/>
+      <c r="B20" s="24">
+        <f>datos!G56</f>
+        <v>0</v>
+      </c>
       <c r="D20" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="24"/>
+      <c r="E20" s="24">
+        <f>datos!G58</f>
+        <v>0</v>
+      </c>
       <c r="F20" s="4"/>
       <c r="G20" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="24"/>
+      <c r="H20" s="24">
+        <f>datos!G60</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="20"/>
+      <c r="B21" s="24">
+        <f>datos!H56</f>
+        <v>0</v>
+      </c>
       <c r="D21" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="20"/>
+      <c r="E21" s="24">
+        <f>datos!H58</f>
+        <v>0</v>
+      </c>
       <c r="F21" s="4"/>
       <c r="G21" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="20"/>
+      <c r="H21" s="24">
+        <f>datos!H60</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
@@ -2915,91 +3464,145 @@
       <c r="A26" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="24"/>
+      <c r="B26" s="24">
+        <f>datos!C62</f>
+        <v>0</v>
+      </c>
       <c r="D26" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="24"/>
+      <c r="E26" s="24">
+        <f>datos!C64</f>
+        <v>0</v>
+      </c>
       <c r="F26" s="4"/>
       <c r="G26" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="24"/>
+      <c r="H26" s="24">
+        <f>datos!C66</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="18"/>
+      <c r="B27" s="24">
+        <f>datos!D62</f>
+        <v>0</v>
+      </c>
       <c r="D27" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="18"/>
+      <c r="E27" s="24">
+        <f>datos!D64</f>
+        <v>0</v>
+      </c>
       <c r="F27" s="4"/>
       <c r="G27" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H27" s="18"/>
+      <c r="H27" s="24">
+        <f>datos!D66</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="24"/>
+      <c r="B28" s="24">
+        <f>datos!E62</f>
+        <v>0</v>
+      </c>
       <c r="D28" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="24"/>
+      <c r="E28" s="24">
+        <f>datos!E64</f>
+        <v>0</v>
+      </c>
       <c r="F28" s="4"/>
       <c r="G28" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="H28" s="24"/>
+      <c r="H28" s="24">
+        <f>datos!E66</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="18"/>
+      <c r="B29" s="24">
+        <f>datos!F62</f>
+        <v>0</v>
+      </c>
       <c r="D29" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="18"/>
+      <c r="E29" s="24">
+        <f>datos!F64</f>
+        <v>0</v>
+      </c>
       <c r="F29" s="4"/>
       <c r="G29" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H29" s="18"/>
+      <c r="H29" s="24">
+        <f>datos!F66</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="24"/>
+      <c r="B30" s="24">
+        <f>datos!G62</f>
+        <v>0</v>
+      </c>
       <c r="D30" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="24"/>
+      <c r="E30" s="24">
+        <f>datos!G64</f>
+        <v>0</v>
+      </c>
       <c r="F30" s="4"/>
       <c r="G30" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H30" s="24"/>
+      <c r="H30" s="24">
+        <f>datos!G66</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="20"/>
+      <c r="B31" s="24">
+        <f>datos!H62</f>
+        <v>0</v>
+      </c>
       <c r="D31" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="20"/>
+      <c r="E31" s="24">
+        <f>datos!H64</f>
+        <v>0</v>
+      </c>
       <c r="F31" s="4"/>
       <c r="G31" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H31" s="20"/>
+      <c r="H31" s="24">
+        <f>datos!H66</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
@@ -3090,91 +3693,145 @@
       <c r="A36" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="24"/>
+      <c r="B36" s="24">
+        <f>datos!C68</f>
+        <v>0</v>
+      </c>
       <c r="D36" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E36" s="24"/>
+      <c r="E36" s="24">
+        <f>datos!C70</f>
+        <v>0</v>
+      </c>
       <c r="F36" s="4"/>
       <c r="G36" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H36" s="24"/>
+      <c r="H36" s="24">
+        <f>datos!C72</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B37" s="18"/>
+      <c r="B37" s="24">
+        <f>datos!D68</f>
+        <v>0</v>
+      </c>
       <c r="D37" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="18"/>
+      <c r="E37" s="24">
+        <f>datos!D70</f>
+        <v>0</v>
+      </c>
       <c r="F37" s="4"/>
       <c r="G37" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H37" s="18"/>
+      <c r="H37" s="24">
+        <f>datos!D72</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="24"/>
+      <c r="B38" s="24">
+        <f>datos!E68</f>
+        <v>0</v>
+      </c>
       <c r="D38" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E38" s="24"/>
+      <c r="E38" s="24">
+        <f>datos!E70</f>
+        <v>0</v>
+      </c>
       <c r="F38" s="4"/>
       <c r="G38" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="H38" s="24"/>
+      <c r="H38" s="24">
+        <f>datos!E72</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="18"/>
+      <c r="B39" s="24">
+        <f>datos!F68</f>
+        <v>0</v>
+      </c>
       <c r="D39" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E39" s="18"/>
+      <c r="E39" s="24">
+        <f>datos!F70</f>
+        <v>0</v>
+      </c>
       <c r="F39" s="4"/>
       <c r="G39" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H39" s="18"/>
+      <c r="H39" s="24">
+        <f>datos!F72</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="24"/>
+      <c r="B40" s="24">
+        <f>datos!G68</f>
+        <v>0</v>
+      </c>
       <c r="D40" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="24"/>
+      <c r="E40" s="24">
+        <f>datos!G70</f>
+        <v>0</v>
+      </c>
       <c r="F40" s="4"/>
       <c r="G40" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H40" s="24"/>
+      <c r="H40" s="24">
+        <f>datos!G72</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="20"/>
+      <c r="B41" s="24">
+        <f>datos!H68</f>
+        <v>0</v>
+      </c>
       <c r="D41" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E41" s="20"/>
+      <c r="E41" s="24">
+        <f>datos!H70</f>
+        <v>0</v>
+      </c>
       <c r="F41" s="4"/>
       <c r="G41" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H41" s="20"/>
+      <c r="H41" s="24">
+        <f>datos!H72</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
@@ -3241,9 +3898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4073,9 +4728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>